<commit_message>
Update uncompleted MorseListening_JJ1SLR_JP.docx and software_component_JP.xlsx
</commit_message>
<xml_diff>
--- a/Document/software_component_JP.xlsx
+++ b/Document/software_component_JP.xlsx
@@ -16,12 +16,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,15 +37,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -62,12 +56,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,9 +91,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,16 +114,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,17 +137,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,15 +161,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,187 +183,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,6 +374,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -408,6 +416,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -419,6 +438,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,41 +469,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -486,148 +479,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -812,12 +805,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>サードパーティのライブラリ</a:t>
+            <a:t>サードパーティの</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>IR</a:t>
@@ -2058,7 +2047,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>初期化</a:t>
+            <a:t>初期化処理</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
         </a:p>
@@ -2670,7 +2659,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>